<commit_message>
From the excel saved in controllers now the functionality is added that save all records from excel to database in machines table
</commit_message>
<xml_diff>
--- a/src/main/java/org/globant/controllers/machines.xlsx
+++ b/src/main/java/org/globant/controllers/machines.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Model</t>
   </si>
@@ -25,7 +25,31 @@
     <t>Impresora</t>
   </si>
   <si>
-    <t>Maquina #D</t>
+    <t>Maquina 3D</t>
+  </si>
+  <si>
+    <t>Escaner</t>
+  </si>
+  <si>
+    <t>Multifuncional Xerox</t>
+  </si>
+  <si>
+    <t>Multifuncional Canon</t>
+  </si>
+  <si>
+    <t>Multifuncional HP</t>
+  </si>
+  <si>
+    <t>Multifuncional Epson</t>
+  </si>
+  <si>
+    <t>Multifuncional Ricoh</t>
+  </si>
+  <si>
+    <t>Multifuncional Brother</t>
+  </si>
+  <si>
+    <t>Multifuncional Samsung</t>
   </si>
 </sst>
 </file>
@@ -284,6 +308,9 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="17.63"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
@@ -317,6 +344,70 @@
         <v>789.0</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="2">
+        <v>1234.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="1">
+        <v>5678.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="1">
+        <v>91011.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="1">
+        <v>1213.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="1">
+        <v>1415.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="1">
+        <v>1617.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="1">
+        <v>1819.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="1">
+        <v>2021.0</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>